<commit_message>
Fillde with the graphs
</commit_message>
<xml_diff>
--- a/output/20141109_cfd60a1_Shootout_fast.xlsx
+++ b/output/20141109_cfd60a1_Shootout_fast.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="193">
   <si>
     <t>criterion</t>
   </si>
@@ -84,471 +84,462 @@
     <t>54</t>
   </si>
   <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>113</t>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>119</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>133</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>148</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
+    <t>154</t>
+  </si>
+  <si>
+    <t>157</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>163</t>
+  </si>
+  <si>
+    <t>166</t>
+  </si>
+  <si>
+    <t>169</t>
+  </si>
+  <si>
+    <t>172</t>
+  </si>
+  <si>
+    <t>175</t>
+  </si>
+  <si>
+    <t>178</t>
+  </si>
+  <si>
+    <t>181</t>
+  </si>
+  <si>
+    <t>184</t>
+  </si>
+  <si>
+    <t>187</t>
+  </si>
+  <si>
+    <t>190</t>
+  </si>
+  <si>
+    <t>193</t>
+  </si>
+  <si>
+    <t>196</t>
+  </si>
+  <si>
+    <t>199</t>
+  </si>
+  <si>
+    <t>202</t>
+  </si>
+  <si>
+    <t>205</t>
+  </si>
+  <si>
+    <t>208</t>
+  </si>
+  <si>
+    <t>211</t>
+  </si>
+  <si>
+    <t>214</t>
+  </si>
+  <si>
+    <t>217</t>
+  </si>
+  <si>
+    <t>220</t>
+  </si>
+  <si>
+    <t>223</t>
+  </si>
+  <si>
+    <t>226</t>
+  </si>
+  <si>
+    <t>229</t>
+  </si>
+  <si>
+    <t>232</t>
+  </si>
+  <si>
+    <t>235</t>
+  </si>
+  <si>
+    <t>238</t>
+  </si>
+  <si>
+    <t>241</t>
+  </si>
+  <si>
+    <t>244</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>Racket</t>
+  </si>
+  <si>
+    <t>Pycket</t>
+  </si>
+  <si>
+    <t>nbody-generic</t>
+  </si>
+  <si>
+    <t>nsieve</t>
+  </si>
+  <si>
+    <t>k-nucleotide</t>
+  </si>
+  <si>
+    <t>ackermann</t>
+  </si>
+  <si>
+    <t>fannkuch</t>
+  </si>
+  <si>
+    <t>meteor</t>
+  </si>
+  <si>
+    <t>binarytrees-generic</t>
+  </si>
+  <si>
+    <t>fannkuch-redux-generic</t>
+  </si>
+  <si>
+    <t>nbody-vec</t>
+  </si>
+  <si>
+    <t>matrix</t>
+  </si>
+  <si>
+    <t>pidigits</t>
+  </si>
+  <si>
+    <t>fasta-generic</t>
+  </si>
+  <si>
+    <t>nbody</t>
+  </si>
+  <si>
+    <t>reversecomplement-generic</t>
+  </si>
+  <si>
+    <t>nestedloop</t>
+  </si>
+  <si>
+    <t>nbody-vec-generic</t>
+  </si>
+  <si>
+    <t>spellcheck</t>
+  </si>
+  <si>
+    <t>partialsums</t>
+  </si>
+  <si>
+    <t>mandelbrot-generic</t>
+  </si>
+  <si>
+    <t>hash</t>
+  </si>
+  <si>
+    <t>ary</t>
+  </si>
+  <si>
+    <t>strcat</t>
+  </si>
+  <si>
+    <t>heapsort</t>
+  </si>
+  <si>
+    <t>fibo</t>
+  </si>
+  <si>
+    <t>recursive</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>regexmatch</t>
+  </si>
+  <si>
+    <t>pidigits1</t>
+  </si>
+  <si>
+    <t>wordfreq</t>
+  </si>
+  <si>
+    <t>moments</t>
+  </si>
+  <si>
+    <t>binarytrees</t>
+  </si>
+  <si>
+    <t>regexpdna</t>
+  </si>
+  <si>
+    <t>fannkuch-redux</t>
+  </si>
+  <si>
+    <t>hash2</t>
+  </si>
+  <si>
+    <t>sieve</t>
+  </si>
+  <si>
+    <t>fasta</t>
+  </si>
+  <si>
+    <t>reversefile</t>
+  </si>
+  <si>
+    <t>nsievebits</t>
+  </si>
+  <si>
+    <t>spectralnorm-generic</t>
+  </si>
+  <si>
+    <t>spectralnorm</t>
+  </si>
+  <si>
+    <t>mandelbrot</t>
+  </si>
+  <si>
+    <t>reversecomplement</t>
+  </si>
+  <si>
+    <t>sumcol</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>mean.norm</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
     <t>57</t>
   </si>
   <si>
-    <t>59</t>
-  </si>
-  <si>
-    <t>62</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
-    <t>68</t>
-  </si>
-  <si>
-    <t>71</t>
-  </si>
-  <si>
-    <t>74</t>
-  </si>
-  <si>
-    <t>77</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>83</t>
-  </si>
-  <si>
-    <t>86</t>
-  </si>
-  <si>
-    <t>89</t>
-  </si>
-  <si>
-    <t>92</t>
-  </si>
-  <si>
-    <t>95</t>
-  </si>
-  <si>
-    <t>98</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>104</t>
-  </si>
-  <si>
-    <t>107</t>
-  </si>
-  <si>
-    <t>110</t>
-  </si>
-  <si>
-    <t>113</t>
-  </si>
-  <si>
-    <t>116</t>
-  </si>
-  <si>
-    <t>119</t>
-  </si>
-  <si>
-    <t>122</t>
-  </si>
-  <si>
-    <t>124</t>
-  </si>
-  <si>
-    <t>130</t>
-  </si>
-  <si>
-    <t>133</t>
-  </si>
-  <si>
-    <t>136</t>
-  </si>
-  <si>
-    <t>139</t>
-  </si>
-  <si>
-    <t>142</t>
-  </si>
-  <si>
-    <t>145</t>
-  </si>
-  <si>
-    <t>148</t>
-  </si>
-  <si>
-    <t>151</t>
-  </si>
-  <si>
-    <t>154</t>
-  </si>
-  <si>
-    <t>157</t>
-  </si>
-  <si>
-    <t>160</t>
-  </si>
-  <si>
-    <t>163</t>
-  </si>
-  <si>
-    <t>166</t>
-  </si>
-  <si>
-    <t>169</t>
-  </si>
-  <si>
-    <t>172</t>
-  </si>
-  <si>
-    <t>175</t>
-  </si>
-  <si>
-    <t>178</t>
-  </si>
-  <si>
-    <t>181</t>
-  </si>
-  <si>
-    <t>184</t>
-  </si>
-  <si>
-    <t>187</t>
-  </si>
-  <si>
-    <t>190</t>
-  </si>
-  <si>
-    <t>193</t>
-  </si>
-  <si>
-    <t>196</t>
-  </si>
-  <si>
-    <t>199</t>
-  </si>
-  <si>
-    <t>202</t>
-  </si>
-  <si>
-    <t>205</t>
-  </si>
-  <si>
-    <t>208</t>
-  </si>
-  <si>
-    <t>211</t>
-  </si>
-  <si>
-    <t>214</t>
-  </si>
-  <si>
-    <t>217</t>
-  </si>
-  <si>
-    <t>220</t>
-  </si>
-  <si>
-    <t>223</t>
-  </si>
-  <si>
-    <t>226</t>
-  </si>
-  <si>
-    <t>229</t>
-  </si>
-  <si>
-    <t>232</t>
-  </si>
-  <si>
-    <t>235</t>
-  </si>
-  <si>
-    <t>238</t>
-  </si>
-  <si>
-    <t>241</t>
-  </si>
-  <si>
-    <t>244</t>
-  </si>
-  <si>
-    <t>247</t>
-  </si>
-  <si>
-    <t>253</t>
-  </si>
-  <si>
-    <t>256</t>
-  </si>
-  <si>
-    <t>total</t>
-  </si>
-  <si>
-    <t>Racket</t>
-  </si>
-  <si>
-    <t>Pycket</t>
-  </si>
-  <si>
-    <t>nbody-generic</t>
-  </si>
-  <si>
-    <t>nsieve</t>
-  </si>
-  <si>
-    <t>lists</t>
-  </si>
-  <si>
-    <t>k-nucleotide</t>
-  </si>
-  <si>
-    <t>ackermann</t>
-  </si>
-  <si>
-    <t>fannkuch</t>
-  </si>
-  <si>
-    <t>meteor</t>
-  </si>
-  <si>
-    <t>binarytrees-generic</t>
-  </si>
-  <si>
-    <t>fannkuch-redux-generic</t>
-  </si>
-  <si>
-    <t>nbody-vec</t>
-  </si>
-  <si>
-    <t>matrix</t>
-  </si>
-  <si>
-    <t>pidigits</t>
-  </si>
-  <si>
-    <t>fasta-generic</t>
-  </si>
-  <si>
-    <t>nbody</t>
-  </si>
-  <si>
-    <t>reversecomplement-generic</t>
-  </si>
-  <si>
-    <t>nestedloop</t>
-  </si>
-  <si>
-    <t>nbody-vec-generic</t>
-  </si>
-  <si>
-    <t>spellcheck</t>
-  </si>
-  <si>
-    <t>partialsums</t>
-  </si>
-  <si>
-    <t>mandelbrot-generic</t>
-  </si>
-  <si>
-    <t>hash</t>
-  </si>
-  <si>
-    <t>ary</t>
-  </si>
-  <si>
-    <t>strcat</t>
-  </si>
-  <si>
-    <t>heapsort</t>
-  </si>
-  <si>
-    <t>fibo</t>
-  </si>
-  <si>
-    <t>recursive</t>
-  </si>
-  <si>
-    <t>random</t>
-  </si>
-  <si>
-    <t>regexmatch</t>
-  </si>
-  <si>
-    <t>pidigits1</t>
-  </si>
-  <si>
-    <t>wordfreq</t>
-  </si>
-  <si>
-    <t>moments</t>
-  </si>
-  <si>
-    <t>binarytrees</t>
-  </si>
-  <si>
-    <t>regexpdna</t>
-  </si>
-  <si>
-    <t>fannkuch-redux</t>
-  </si>
-  <si>
-    <t>hash2</t>
-  </si>
-  <si>
-    <t>sieve</t>
-  </si>
-  <si>
-    <t>fasta</t>
-  </si>
-  <si>
-    <t>reversefile</t>
-  </si>
-  <si>
-    <t>nsievebits</t>
-  </si>
-  <si>
-    <t>spectralnorm-generic</t>
-  </si>
-  <si>
-    <t>spectralnorm</t>
-  </si>
-  <si>
-    <t>mandelbrot</t>
-  </si>
-  <si>
-    <t>reversecomplement</t>
-  </si>
-  <si>
-    <t>sumcol</t>
-  </si>
-  <si>
-    <t>overall</t>
-  </si>
-  <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>median</t>
-  </si>
-  <si>
-    <t>mean.norm</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>52</t>
-  </si>
-  <si>
-    <t>53</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>56</t>
-  </si>
-  <si>
     <t>58</t>
   </si>
   <si>
@@ -598,9 +589,6 @@
   </si>
   <si>
     <t>82</t>
-  </si>
-  <si>
-    <t>84</t>
   </si>
   <si>
     <t>FALSE</t>
@@ -677,13 +665,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" t="s">
         <v>90</v>
-      </c>
-      <c r="D2" t="s">
-        <v>92</v>
       </c>
       <c r="E2" t="n">
         <v>8877.0</v>
@@ -697,13 +685,13 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E3" t="n">
         <v>15122.0</v>
@@ -717,16 +705,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E4" t="n">
-        <v>5314.0</v>
+        <v>2929.0</v>
       </c>
       <c r="F4" t="e">
         <v>#N/A</v>
@@ -737,16 +725,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E5" t="n">
-        <v>2929.0</v>
+        <v>5327.0</v>
       </c>
       <c r="F5" t="e">
         <v>#N/A</v>
@@ -757,16 +745,16 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E6" t="n">
-        <v>5327.0</v>
+        <v>2180.0</v>
       </c>
       <c r="F6" t="e">
         <v>#N/A</v>
@@ -777,16 +765,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E7" t="n">
-        <v>2180.0</v>
+        <v>395.0</v>
       </c>
       <c r="F7" t="e">
         <v>#N/A</v>
@@ -797,16 +785,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E8" t="n">
-        <v>395.0</v>
+        <v>2198.0</v>
       </c>
       <c r="F8" t="e">
         <v>#N/A</v>
@@ -817,16 +805,16 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E9" t="n">
-        <v>2198.0</v>
+        <v>2163.0</v>
       </c>
       <c r="F9" t="e">
         <v>#N/A</v>
@@ -837,16 +825,16 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E10" t="n">
-        <v>2163.0</v>
+        <v>2195.0</v>
       </c>
       <c r="F10" t="e">
         <v>#N/A</v>
@@ -857,16 +845,16 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E11" t="n">
-        <v>2195.0</v>
+        <v>4843.0</v>
       </c>
       <c r="F11" t="e">
         <v>#N/A</v>
@@ -877,16 +865,16 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E12" t="n">
-        <v>4843.0</v>
+        <v>1547.0</v>
       </c>
       <c r="F12" t="e">
         <v>#N/A</v>
@@ -897,16 +885,16 @@
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E13" t="n">
-        <v>1547.0</v>
+        <v>3196.0</v>
       </c>
       <c r="F13" t="e">
         <v>#N/A</v>
@@ -917,16 +905,16 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E14" t="n">
-        <v>3196.0</v>
+        <v>4186.0</v>
       </c>
       <c r="F14" t="e">
         <v>#N/A</v>
@@ -937,16 +925,16 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E15" t="n">
-        <v>4186.0</v>
+        <v>8618.0</v>
       </c>
       <c r="F15" t="e">
         <v>#N/A</v>
@@ -957,16 +945,16 @@
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E16" t="n">
-        <v>8618.0</v>
+        <v>7527.0</v>
       </c>
       <c r="F16" t="e">
         <v>#N/A</v>
@@ -977,16 +965,16 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E17" t="n">
-        <v>7527.0</v>
+        <v>8875.0</v>
       </c>
       <c r="F17" t="e">
         <v>#N/A</v>
@@ -997,16 +985,16 @@
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D18" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E18" t="n">
-        <v>8875.0</v>
+        <v>916.0</v>
       </c>
       <c r="F18" t="e">
         <v>#N/A</v>
@@ -1017,16 +1005,16 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E19" t="n">
-        <v>916.0</v>
+        <v>3060.0</v>
       </c>
       <c r="F19" t="e">
         <v>#N/A</v>
@@ -1037,16 +1025,16 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E20" t="n">
-        <v>3060.0</v>
+        <v>11607.0</v>
       </c>
       <c r="F20" t="e">
         <v>#N/A</v>
@@ -1057,16 +1045,16 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D21" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E21" t="n">
-        <v>11607.0</v>
+        <v>5405.0</v>
       </c>
       <c r="F21" t="e">
         <v>#N/A</v>
@@ -1077,16 +1065,16 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D22" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E22" t="n">
-        <v>5405.0</v>
+        <v>7255.0</v>
       </c>
       <c r="F22" t="e">
         <v>#N/A</v>
@@ -1097,16 +1085,16 @@
         <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D23" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E23" t="n">
-        <v>7255.0</v>
+        <v>3170.0</v>
       </c>
       <c r="F23" t="e">
         <v>#N/A</v>
@@ -1117,16 +1105,16 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D24" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E24" t="n">
-        <v>3170.0</v>
+        <v>5879.0</v>
       </c>
       <c r="F24" t="e">
         <v>#N/A</v>
@@ -1137,16 +1125,16 @@
         <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D25" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E25" t="n">
-        <v>5879.0</v>
+        <v>5516.0</v>
       </c>
       <c r="F25" t="e">
         <v>#N/A</v>
@@ -1157,16 +1145,16 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D26" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E26" t="n">
-        <v>5516.0</v>
+        <v>10921.0</v>
       </c>
       <c r="F26" t="e">
         <v>#N/A</v>
@@ -1177,16 +1165,16 @@
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D27" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E27" t="n">
-        <v>10921.0</v>
+        <v>3469.0</v>
       </c>
       <c r="F27" t="e">
         <v>#N/A</v>
@@ -1197,16 +1185,16 @@
         <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D28" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E28" t="n">
-        <v>3469.0</v>
+        <v>4341.0</v>
       </c>
       <c r="F28" t="e">
         <v>#N/A</v>
@@ -1217,16 +1205,16 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D29" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E29" t="n">
-        <v>4341.0</v>
+        <v>565.0</v>
       </c>
       <c r="F29" t="e">
         <v>#N/A</v>
@@ -1237,16 +1225,16 @@
         <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D30" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E30" t="n">
-        <v>565.0</v>
+        <v>4033.0</v>
       </c>
       <c r="F30" t="e">
         <v>#N/A</v>
@@ -1257,16 +1245,16 @@
         <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C31" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D31" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E31" t="n">
-        <v>4033.0</v>
+        <v>5353.0</v>
       </c>
       <c r="F31" t="e">
         <v>#N/A</v>
@@ -1277,16 +1265,16 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C32" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E32" t="n">
-        <v>5353.0</v>
+        <v>1837.0</v>
       </c>
       <c r="F32" t="e">
         <v>#N/A</v>
@@ -1297,16 +1285,16 @@
         <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D33" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E33" t="n">
-        <v>1837.0</v>
+        <v>6784.0</v>
       </c>
       <c r="F33" t="e">
         <v>#N/A</v>
@@ -1317,16 +1305,16 @@
         <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D34" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E34" t="n">
-        <v>6784.0</v>
+        <v>1524.0</v>
       </c>
       <c r="F34" t="e">
         <v>#N/A</v>
@@ -1337,16 +1325,16 @@
         <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C35" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D35" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E35" t="n">
-        <v>1524.0</v>
+        <v>3093.0</v>
       </c>
       <c r="F35" t="e">
         <v>#N/A</v>
@@ -1357,16 +1345,16 @@
         <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D36" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E36" t="n">
-        <v>3093.0</v>
+        <v>6215.0</v>
       </c>
       <c r="F36" t="e">
         <v>#N/A</v>
@@ -1377,16 +1365,16 @@
         <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C37" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D37" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E37" t="n">
-        <v>6215.0</v>
+        <v>3379.0</v>
       </c>
       <c r="F37" t="e">
         <v>#N/A</v>
@@ -1397,16 +1385,16 @@
         <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C38" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D38" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E38" t="n">
-        <v>3379.0</v>
+        <v>2295.0</v>
       </c>
       <c r="F38" t="e">
         <v>#N/A</v>
@@ -1417,16 +1405,16 @@
         <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C39" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D39" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E39" t="n">
-        <v>2295.0</v>
+        <v>6296.0</v>
       </c>
       <c r="F39" t="e">
         <v>#N/A</v>
@@ -1437,16 +1425,16 @@
         <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C40" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D40" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E40" t="n">
-        <v>6296.0</v>
+        <v>14088.0</v>
       </c>
       <c r="F40" t="e">
         <v>#N/A</v>
@@ -1457,16 +1445,16 @@
         <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C41" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D41" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E41" t="n">
-        <v>14088.0</v>
+        <v>1770.0</v>
       </c>
       <c r="F41" t="e">
         <v>#N/A</v>
@@ -1477,16 +1465,16 @@
         <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C42" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D42" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E42" t="n">
-        <v>1770.0</v>
+        <v>2347.0</v>
       </c>
       <c r="F42" t="e">
         <v>#N/A</v>
@@ -1497,16 +1485,16 @@
         <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C43" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D43" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E43" t="n">
-        <v>2347.0</v>
+        <v>5504.0</v>
       </c>
       <c r="F43" t="e">
         <v>#N/A</v>
@@ -1517,16 +1505,16 @@
         <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C44" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D44" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E44" t="n">
-        <v>5504.0</v>
+        <v>3269.0</v>
       </c>
       <c r="F44" t="e">
         <v>#N/A</v>
@@ -1537,16 +1525,16 @@
         <v>48</v>
       </c>
       <c r="B45" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C45" t="s">
+        <v>89</v>
+      </c>
+      <c r="D45" t="s">
         <v>90</v>
       </c>
-      <c r="D45" t="s">
-        <v>135</v>
-      </c>
       <c r="E45" t="n">
-        <v>3269.0</v>
+        <v>2136.0</v>
       </c>
       <c r="F45" t="e">
         <v>#N/A</v>
@@ -1557,16 +1545,16 @@
         <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C46" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D46" t="s">
-        <v>92</v>
+        <v>123</v>
       </c>
       <c r="E46" t="n">
-        <v>2136.0</v>
+        <v>1096.0</v>
       </c>
       <c r="F46" t="e">
         <v>#N/A</v>
@@ -1577,16 +1565,16 @@
         <v>50</v>
       </c>
       <c r="B47" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C47" t="s">
+        <v>89</v>
+      </c>
+      <c r="D47" t="s">
         <v>91</v>
       </c>
-      <c r="D47" t="s">
-        <v>126</v>
-      </c>
       <c r="E47" t="n">
-        <v>1096.0</v>
+        <v>4748.0</v>
       </c>
       <c r="F47" t="e">
         <v>#N/A</v>
@@ -1597,16 +1585,16 @@
         <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C48" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D48" t="s">
         <v>93</v>
       </c>
       <c r="E48" t="n">
-        <v>4748.0</v>
+        <v>6016.0</v>
       </c>
       <c r="F48" t="e">
         <v>#N/A</v>
@@ -1617,16 +1605,16 @@
         <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C49" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D49" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E49" t="n">
-        <v>6016.0</v>
+        <v>1476.0</v>
       </c>
       <c r="F49" t="e">
         <v>#N/A</v>
@@ -1637,16 +1625,16 @@
         <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C50" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D50" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E50" t="n">
-        <v>1476.0</v>
+        <v>920.0</v>
       </c>
       <c r="F50" t="e">
         <v>#N/A</v>
@@ -1657,16 +1645,16 @@
         <v>54</v>
       </c>
       <c r="B51" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C51" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D51" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E51" t="n">
-        <v>920.0</v>
+        <v>3240.0</v>
       </c>
       <c r="F51" t="e">
         <v>#N/A</v>
@@ -1677,16 +1665,16 @@
         <v>55</v>
       </c>
       <c r="B52" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C52" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D52" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E52" t="n">
-        <v>3240.0</v>
+        <v>1584.0</v>
       </c>
       <c r="F52" t="e">
         <v>#N/A</v>
@@ -1697,16 +1685,16 @@
         <v>56</v>
       </c>
       <c r="B53" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C53" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E53" t="n">
-        <v>1584.0</v>
+        <v>2284.0</v>
       </c>
       <c r="F53" t="e">
         <v>#N/A</v>
@@ -1717,16 +1705,16 @@
         <v>57</v>
       </c>
       <c r="B54" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C54" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D54" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E54" t="n">
-        <v>2284.0</v>
+        <v>1688.0</v>
       </c>
       <c r="F54" t="e">
         <v>#N/A</v>
@@ -1737,16 +1725,16 @@
         <v>58</v>
       </c>
       <c r="B55" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C55" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D55" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E55" t="n">
-        <v>1688.0</v>
+        <v>12296.0</v>
       </c>
       <c r="F55" t="e">
         <v>#N/A</v>
@@ -1757,16 +1745,16 @@
         <v>59</v>
       </c>
       <c r="B56" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C56" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D56" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E56" t="n">
-        <v>12296.0</v>
+        <v>2088.0</v>
       </c>
       <c r="F56" t="e">
         <v>#N/A</v>
@@ -1777,16 +1765,16 @@
         <v>60</v>
       </c>
       <c r="B57" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C57" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E57" t="n">
-        <v>2088.0</v>
+        <v>3040.0</v>
       </c>
       <c r="F57" t="e">
         <v>#N/A</v>
@@ -1797,16 +1785,16 @@
         <v>61</v>
       </c>
       <c r="B58" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C58" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D58" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E58" t="n">
-        <v>3040.0</v>
+        <v>1492.0</v>
       </c>
       <c r="F58" t="e">
         <v>#N/A</v>
@@ -1817,16 +1805,16 @@
         <v>62</v>
       </c>
       <c r="B59" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C59" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D59" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E59" t="n">
-        <v>1492.0</v>
+        <v>1064.0</v>
       </c>
       <c r="F59" t="e">
         <v>#N/A</v>
@@ -1837,16 +1825,16 @@
         <v>63</v>
       </c>
       <c r="B60" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C60" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D60" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E60" t="n">
-        <v>1064.0</v>
+        <v>980.0</v>
       </c>
       <c r="F60" t="e">
         <v>#N/A</v>
@@ -1857,16 +1845,16 @@
         <v>64</v>
       </c>
       <c r="B61" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C61" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D61" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E61" t="n">
-        <v>980.0</v>
+        <v>2368.0</v>
       </c>
       <c r="F61" t="e">
         <v>#N/A</v>
@@ -1877,16 +1865,16 @@
         <v>65</v>
       </c>
       <c r="B62" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C62" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D62" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E62" t="n">
-        <v>2368.0</v>
+        <v>1692.0</v>
       </c>
       <c r="F62" t="e">
         <v>#N/A</v>
@@ -1897,16 +1885,16 @@
         <v>66</v>
       </c>
       <c r="B63" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C63" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D63" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E63" t="n">
-        <v>1692.0</v>
+        <v>2500.0</v>
       </c>
       <c r="F63" t="e">
         <v>#N/A</v>
@@ -1917,16 +1905,16 @@
         <v>67</v>
       </c>
       <c r="B64" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C64" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D64" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E64" t="n">
-        <v>2500.0</v>
+        <v>8040.0</v>
       </c>
       <c r="F64" t="e">
         <v>#N/A</v>
@@ -1937,16 +1925,16 @@
         <v>68</v>
       </c>
       <c r="B65" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C65" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D65" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E65" t="n">
-        <v>8040.0</v>
+        <v>11884.0</v>
       </c>
       <c r="F65" t="e">
         <v>#N/A</v>
@@ -1957,16 +1945,16 @@
         <v>69</v>
       </c>
       <c r="B66" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C66" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D66" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E66" t="n">
-        <v>11884.0</v>
+        <v>860.0</v>
       </c>
       <c r="F66" t="e">
         <v>#N/A</v>
@@ -1977,16 +1965,16 @@
         <v>70</v>
       </c>
       <c r="B67" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C67" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D67" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E67" t="n">
-        <v>860.0</v>
+        <v>2776.0</v>
       </c>
       <c r="F67" t="e">
         <v>#N/A</v>
@@ -1997,16 +1985,16 @@
         <v>71</v>
       </c>
       <c r="B68" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C68" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D68" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E68" t="n">
-        <v>2776.0</v>
+        <v>208.0</v>
       </c>
       <c r="F68" t="e">
         <v>#N/A</v>
@@ -2017,16 +2005,16 @@
         <v>72</v>
       </c>
       <c r="B69" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D69" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="E69" t="n">
-        <v>208.0</v>
+        <v>12892.0</v>
       </c>
       <c r="F69" t="e">
         <v>#N/A</v>
@@ -2037,16 +2025,16 @@
         <v>73</v>
       </c>
       <c r="B70" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C70" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D70" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="E70" t="n">
-        <v>12892.0</v>
+        <v>4880.0</v>
       </c>
       <c r="F70" t="e">
         <v>#N/A</v>
@@ -2057,16 +2045,16 @@
         <v>74</v>
       </c>
       <c r="B71" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C71" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D71" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E71" t="n">
-        <v>4880.0</v>
+        <v>3180.0</v>
       </c>
       <c r="F71" t="e">
         <v>#N/A</v>
@@ -2077,16 +2065,16 @@
         <v>75</v>
       </c>
       <c r="B72" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C72" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D72" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="E72" t="n">
-        <v>3180.0</v>
+        <v>4944.0</v>
       </c>
       <c r="F72" t="e">
         <v>#N/A</v>
@@ -2097,16 +2085,16 @@
         <v>76</v>
       </c>
       <c r="B73" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C73" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D73" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="E73" t="n">
-        <v>4944.0</v>
+        <v>1504.0</v>
       </c>
       <c r="F73" t="e">
         <v>#N/A</v>
@@ -2117,16 +2105,16 @@
         <v>77</v>
       </c>
       <c r="B74" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C74" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D74" t="s">
-        <v>125</v>
+        <v>98</v>
       </c>
       <c r="E74" t="n">
-        <v>1504.0</v>
+        <v>1256.0</v>
       </c>
       <c r="F74" t="e">
         <v>#N/A</v>
@@ -2137,16 +2125,16 @@
         <v>78</v>
       </c>
       <c r="B75" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C75" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D75" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="E75" t="n">
-        <v>1256.0</v>
+        <v>2480.0</v>
       </c>
       <c r="F75" t="e">
         <v>#N/A</v>
@@ -2157,16 +2145,16 @@
         <v>79</v>
       </c>
       <c r="B76" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C76" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D76" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="E76" t="n">
-        <v>2480.0</v>
+        <v>1488.0</v>
       </c>
       <c r="F76" t="e">
         <v>#N/A</v>
@@ -2177,16 +2165,16 @@
         <v>80</v>
       </c>
       <c r="B77" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C77" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D77" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E77" t="n">
-        <v>1488.0</v>
+        <v>4368.0</v>
       </c>
       <c r="F77" t="e">
         <v>#N/A</v>
@@ -2197,16 +2185,16 @@
         <v>81</v>
       </c>
       <c r="B78" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C78" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D78" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="E78" t="n">
-        <v>4368.0</v>
+        <v>8916.0</v>
       </c>
       <c r="F78" t="e">
         <v>#N/A</v>
@@ -2217,16 +2205,16 @@
         <v>82</v>
       </c>
       <c r="B79" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C79" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D79" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E79" t="n">
-        <v>8916.0</v>
+        <v>1192.0</v>
       </c>
       <c r="F79" t="e">
         <v>#N/A</v>
@@ -2237,16 +2225,16 @@
         <v>83</v>
       </c>
       <c r="B80" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C80" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D80" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E80" t="n">
-        <v>1192.0</v>
+        <v>2424.0</v>
       </c>
       <c r="F80" t="e">
         <v>#N/A</v>
@@ -2257,16 +2245,16 @@
         <v>84</v>
       </c>
       <c r="B81" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C81" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D81" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E81" t="n">
-        <v>2424.0</v>
+        <v>2588.0</v>
       </c>
       <c r="F81" t="e">
         <v>#N/A</v>
@@ -2277,16 +2265,16 @@
         <v>85</v>
       </c>
       <c r="B82" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C82" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D82" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E82" t="n">
-        <v>2588.0</v>
+        <v>2136.0</v>
       </c>
       <c r="F82" t="e">
         <v>#N/A</v>
@@ -2297,58 +2285,18 @@
         <v>86</v>
       </c>
       <c r="B83" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C83" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D83" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E83" t="n">
-        <v>2136.0</v>
+        <v>1216.0</v>
       </c>
       <c r="F83" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="s">
-        <v>87</v>
-      </c>
-      <c r="B84" t="s">
-        <v>89</v>
-      </c>
-      <c r="C84" t="s">
-        <v>91</v>
-      </c>
-      <c r="D84" t="s">
-        <v>135</v>
-      </c>
-      <c r="E84" t="n">
-        <v>1216.0</v>
-      </c>
-      <c r="F84" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="s">
-        <v>88</v>
-      </c>
-      <c r="B85" t="s">
-        <v>89</v>
-      </c>
-      <c r="C85" t="s">
-        <v>91</v>
-      </c>
-      <c r="D85" t="s">
-        <v>94</v>
-      </c>
-      <c r="E85" t="n">
-        <v>2179988.0</v>
-      </c>
-      <c r="F85" t="e">
         <v>#N/A</v>
       </c>
     </row>
@@ -2374,30 +2322,30 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G1" t="s">
         <v>136</v>
-      </c>
-      <c r="E1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E2" t="n">
         <v>6016.0</v>
@@ -2411,16 +2359,16 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E3" t="n">
         <v>5327.0</v>
@@ -2437,13 +2385,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E4" t="n">
         <v>1692.0</v>
@@ -2457,16 +2405,16 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D5" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E5" t="n">
         <v>7255.0</v>
@@ -2480,16 +2428,16 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E6" t="n">
         <v>3180.0</v>
@@ -2506,13 +2454,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D7" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E7" t="n">
         <v>1837.0</v>
@@ -2526,16 +2474,16 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D8" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E8" t="n">
         <v>3240.0</v>
@@ -2549,16 +2497,16 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D9" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E9" t="n">
         <v>2198.0</v>
@@ -2575,13 +2523,13 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D10" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E10" t="n">
         <v>1476.0</v>
@@ -2595,16 +2543,16 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D11" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E11" t="n">
         <v>2180.0</v>
@@ -2618,16 +2566,16 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B12" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D12" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E12" t="n">
         <v>1504.0</v>
@@ -2644,13 +2592,13 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D13" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E13" t="n">
         <v>1524.0</v>
@@ -2664,16 +2612,16 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B14" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D14" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E14" t="n">
         <v>1584.0</v>
@@ -2687,16 +2635,16 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D15" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E15" t="n">
         <v>2163.0</v>
@@ -2713,13 +2661,13 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D16" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E16" t="n">
         <v>12892.0</v>
@@ -2733,16 +2681,16 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B17" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D17" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E17" t="n">
         <v>3379.0</v>
@@ -2756,16 +2704,16 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B18" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D18" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E18" t="n">
         <v>12296.0</v>
@@ -2782,13 +2730,13 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D19" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E19" t="n">
         <v>3196.0</v>
@@ -2802,16 +2750,16 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B20" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D20" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E20" t="n">
         <v>4944.0</v>
@@ -2825,16 +2773,16 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B21" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D21" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E21" t="n">
         <v>5516.0</v>
@@ -2851,13 +2799,13 @@
         <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D22" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E22" t="n">
         <v>2776.0</v>
@@ -2871,16 +2819,16 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D23" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E23" t="n">
         <v>5405.0</v>
@@ -2894,16 +2842,16 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C24" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D24" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E24" t="n">
         <v>1096.0</v>
@@ -2920,13 +2868,13 @@
         <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D25" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E25" t="n">
         <v>3093.0</v>
@@ -2940,16 +2888,16 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B26" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D26" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E26" t="n">
         <v>8040.0</v>
@@ -2963,16 +2911,16 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B27" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D27" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E27" t="n">
         <v>5879.0</v>
@@ -2989,13 +2937,13 @@
         <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D28" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E28" t="n">
         <v>2929.0</v>
@@ -3009,45 +2957,45 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>130</v>
       </c>
       <c r="C29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D29" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E29" t="n">
-        <v>2179988.0</v>
+        <v>2136.0</v>
       </c>
       <c r="F29" t="n">
-        <v>2179988.0</v>
+        <v>2136.0</v>
       </c>
       <c r="G29" t="n">
-        <v>410.23485133609336</v>
+        <v>0.9100979974435449</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>130</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D30" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E30" t="n">
-        <v>5314.0</v>
+        <v>2347.0</v>
       </c>
       <c r="F30" t="n">
-        <v>5314.0</v>
+        <v>2347.0</v>
       </c>
       <c r="G30" t="n">
         <v>1.0</v>
@@ -3058,42 +3006,42 @@
         <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="C31" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D31" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E31" t="n">
-        <v>2136.0</v>
+        <v>2368.0</v>
       </c>
       <c r="F31" t="n">
-        <v>2136.0</v>
+        <v>2368.0</v>
       </c>
       <c r="G31" t="n">
-        <v>0.9100979974435449</v>
+        <v>0.20401481864392176</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B32" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="C32" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D32" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E32" t="n">
-        <v>2347.0</v>
+        <v>11607.0</v>
       </c>
       <c r="F32" t="n">
-        <v>2347.0</v>
+        <v>11607.0</v>
       </c>
       <c r="G32" t="n">
         <v>1.0</v>
@@ -3101,25 +3049,25 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B33" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D33" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E33" t="n">
-        <v>2368.0</v>
+        <v>2284.0</v>
       </c>
       <c r="F33" t="n">
-        <v>2368.0</v>
+        <v>2284.0</v>
       </c>
       <c r="G33" t="n">
-        <v>0.20401481864392176</v>
+        <v>0.4716085071236837</v>
       </c>
     </row>
     <row r="34">
@@ -3127,19 +3075,19 @@
         <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D34" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E34" t="n">
-        <v>11607.0</v>
+        <v>4843.0</v>
       </c>
       <c r="F34" t="n">
-        <v>11607.0</v>
+        <v>4843.0</v>
       </c>
       <c r="G34" t="n">
         <v>1.0</v>
@@ -3147,45 +3095,45 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C35" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D35" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E35" t="n">
-        <v>2284.0</v>
+        <v>920.0</v>
       </c>
       <c r="F35" t="n">
-        <v>2284.0</v>
+        <v>920.0</v>
       </c>
       <c r="G35" t="n">
-        <v>0.4716085071236837</v>
+        <v>2.329113924050633</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B36" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D36" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E36" t="n">
-        <v>4843.0</v>
+        <v>395.0</v>
       </c>
       <c r="F36" t="n">
-        <v>4843.0</v>
+        <v>395.0</v>
       </c>
       <c r="G36" t="n">
         <v>1.0</v>
@@ -3196,42 +3144,42 @@
         <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="C37" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D37" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E37" t="n">
-        <v>920.0</v>
+        <v>4880.0</v>
       </c>
       <c r="F37" t="n">
-        <v>920.0</v>
+        <v>4880.0</v>
       </c>
       <c r="G37" t="n">
-        <v>2.329113924050633</v>
+        <v>0.9116383336446853</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B38" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="C38" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D38" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E38" t="n">
-        <v>395.0</v>
+        <v>5353.0</v>
       </c>
       <c r="F38" t="n">
-        <v>395.0</v>
+        <v>5353.0</v>
       </c>
       <c r="G38" t="n">
         <v>1.0</v>
@@ -3239,25 +3187,25 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B39" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C39" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D39" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E39" t="n">
-        <v>4880.0</v>
+        <v>2088.0</v>
       </c>
       <c r="F39" t="n">
-        <v>4880.0</v>
+        <v>2088.0</v>
       </c>
       <c r="G39" t="n">
-        <v>0.9116383336446853</v>
+        <v>0.49880554228380314</v>
       </c>
     </row>
     <row r="40">
@@ -3265,19 +3213,19 @@
         <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C40" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D40" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E40" t="n">
-        <v>5353.0</v>
+        <v>4186.0</v>
       </c>
       <c r="F40" t="n">
-        <v>5353.0</v>
+        <v>4186.0</v>
       </c>
       <c r="G40" t="n">
         <v>1.0</v>
@@ -3285,45 +3233,45 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B41" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="C41" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D41" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E41" t="n">
-        <v>2088.0</v>
+        <v>2136.0</v>
       </c>
       <c r="F41" t="n">
-        <v>2088.0</v>
+        <v>2136.0</v>
       </c>
       <c r="G41" t="n">
-        <v>0.49880554228380314</v>
+        <v>0.24062183169989862</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B42" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="C42" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D42" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E42" t="n">
-        <v>4186.0</v>
+        <v>8877.0</v>
       </c>
       <c r="F42" t="n">
-        <v>4186.0</v>
+        <v>8877.0</v>
       </c>
       <c r="G42" t="n">
         <v>1.0</v>
@@ -3334,42 +3282,42 @@
         <v>18</v>
       </c>
       <c r="B43" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C43" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D43" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E43" t="n">
-        <v>2136.0</v>
+        <v>1256.0</v>
       </c>
       <c r="F43" t="n">
-        <v>2136.0</v>
+        <v>1256.0</v>
       </c>
       <c r="G43" t="n">
-        <v>0.24062183169989862</v>
+        <v>0.5722095671981777</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B44" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C44" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D44" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E44" t="n">
-        <v>8877.0</v>
+        <v>2195.0</v>
       </c>
       <c r="F44" t="n">
-        <v>8877.0</v>
+        <v>2195.0</v>
       </c>
       <c r="G44" t="n">
         <v>1.0</v>
@@ -3377,25 +3325,25 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B45" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C45" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D45" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E45" t="n">
-        <v>1256.0</v>
+        <v>1492.0</v>
       </c>
       <c r="F45" t="n">
-        <v>1256.0</v>
+        <v>1492.0</v>
       </c>
       <c r="G45" t="n">
-        <v>0.5722095671981777</v>
+        <v>0.16811267605633803</v>
       </c>
     </row>
     <row r="46">
@@ -3403,19 +3351,19 @@
         <v>19</v>
       </c>
       <c r="B46" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C46" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D46" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E46" t="n">
-        <v>2195.0</v>
+        <v>8875.0</v>
       </c>
       <c r="F46" t="n">
-        <v>2195.0</v>
+        <v>8875.0</v>
       </c>
       <c r="G46" t="n">
         <v>1.0</v>
@@ -3423,45 +3371,45 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B47" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C47" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D47" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E47" t="n">
-        <v>1492.0</v>
+        <v>3040.0</v>
       </c>
       <c r="F47" t="n">
-        <v>1492.0</v>
+        <v>3040.0</v>
       </c>
       <c r="G47" t="n">
-        <v>0.16811267605633803</v>
+        <v>0.40387936760993753</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B48" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C48" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D48" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E48" t="n">
-        <v>8875.0</v>
+        <v>7527.0</v>
       </c>
       <c r="F48" t="n">
-        <v>8875.0</v>
+        <v>7527.0</v>
       </c>
       <c r="G48" t="n">
         <v>1.0</v>
@@ -3472,42 +3420,42 @@
         <v>20</v>
       </c>
       <c r="B49" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="C49" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D49" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E49" t="n">
-        <v>3040.0</v>
+        <v>4748.0</v>
       </c>
       <c r="F49" t="n">
-        <v>3040.0</v>
+        <v>4748.0</v>
       </c>
       <c r="G49" t="n">
-        <v>0.40387936760993753</v>
+        <v>0.3139796323237667</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B50" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="C50" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D50" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E50" t="n">
-        <v>7527.0</v>
+        <v>15122.0</v>
       </c>
       <c r="F50" t="n">
-        <v>7527.0</v>
+        <v>15122.0</v>
       </c>
       <c r="G50" t="n">
         <v>1.0</v>
@@ -3515,25 +3463,25 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B51" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="C51" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D51" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E51" t="n">
-        <v>4748.0</v>
+        <v>1192.0</v>
       </c>
       <c r="F51" t="n">
-        <v>4748.0</v>
+        <v>1192.0</v>
       </c>
       <c r="G51" t="n">
-        <v>0.3139796323237667</v>
+        <v>0.18932655654383734</v>
       </c>
     </row>
     <row r="52">
@@ -3541,19 +3489,19 @@
         <v>21</v>
       </c>
       <c r="B52" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="C52" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D52" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E52" t="n">
-        <v>15122.0</v>
+        <v>6296.0</v>
       </c>
       <c r="F52" t="n">
-        <v>15122.0</v>
+        <v>6296.0</v>
       </c>
       <c r="G52" t="n">
         <v>1.0</v>
@@ -3561,45 +3509,45 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B53" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="C53" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D53" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E53" t="n">
-        <v>1192.0</v>
+        <v>980.0</v>
       </c>
       <c r="F53" t="n">
-        <v>1192.0</v>
+        <v>980.0</v>
       </c>
       <c r="G53" t="n">
-        <v>0.18932655654383734</v>
+        <v>0.3202614379084967</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B54" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="C54" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D54" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E54" t="n">
-        <v>6296.0</v>
+        <v>3060.0</v>
       </c>
       <c r="F54" t="n">
-        <v>6296.0</v>
+        <v>3060.0</v>
       </c>
       <c r="G54" t="n">
         <v>1.0</v>
@@ -3610,42 +3558,42 @@
         <v>22</v>
       </c>
       <c r="B55" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C55" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D55" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E55" t="n">
-        <v>980.0</v>
+        <v>1688.0</v>
       </c>
       <c r="F55" t="n">
-        <v>980.0</v>
+        <v>1688.0</v>
       </c>
       <c r="G55" t="n">
-        <v>0.3202614379084967</v>
+        <v>1.0911441499676793</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B56" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C56" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D56" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E56" t="n">
-        <v>3060.0</v>
+        <v>1547.0</v>
       </c>
       <c r="F56" t="n">
-        <v>3060.0</v>
+        <v>1547.0</v>
       </c>
       <c r="G56" t="n">
         <v>1.0</v>
@@ -3653,45 +3601,45 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>177</v>
+        <v>23</v>
       </c>
       <c r="B57" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="C57" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D57" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E57" t="n">
-        <v>1688.0</v>
+        <v>208.0</v>
       </c>
       <c r="F57" t="n">
-        <v>1688.0</v>
+        <v>208.0</v>
       </c>
       <c r="G57" t="n">
-        <v>1.0911441499676793</v>
+        <v>0.368141592920354</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>23</v>
+        <v>174</v>
       </c>
       <c r="B58" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="C58" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D58" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E58" t="n">
-        <v>1547.0</v>
+        <v>565.0</v>
       </c>
       <c r="F58" t="n">
-        <v>1547.0</v>
+        <v>565.0</v>
       </c>
       <c r="G58" t="n">
         <v>1.0</v>
@@ -3699,25 +3647,25 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B59" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C59" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D59" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E59" t="n">
-        <v>208.0</v>
+        <v>860.0</v>
       </c>
       <c r="F59" t="n">
-        <v>208.0</v>
+        <v>860.0</v>
       </c>
       <c r="G59" t="n">
-        <v>0.368141592920354</v>
+        <v>0.24791006053617756</v>
       </c>
     </row>
     <row r="60">
@@ -3725,19 +3673,19 @@
         <v>24</v>
       </c>
       <c r="B60" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C60" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D60" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E60" t="n">
-        <v>565.0</v>
+        <v>3469.0</v>
       </c>
       <c r="F60" t="n">
-        <v>565.0</v>
+        <v>3469.0</v>
       </c>
       <c r="G60" t="n">
         <v>1.0</v>
@@ -3745,45 +3693,45 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B61" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C61" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D61" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E61" t="n">
-        <v>860.0</v>
+        <v>11884.0</v>
       </c>
       <c r="F61" t="n">
-        <v>860.0</v>
+        <v>11884.0</v>
       </c>
       <c r="G61" t="n">
-        <v>0.24791006053617756</v>
+        <v>1.0881787382107866</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B62" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C62" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D62" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E62" t="n">
-        <v>3469.0</v>
+        <v>10921.0</v>
       </c>
       <c r="F62" t="n">
-        <v>3469.0</v>
+        <v>10921.0</v>
       </c>
       <c r="G62" t="n">
         <v>1.0</v>
@@ -3794,42 +3742,42 @@
         <v>25</v>
       </c>
       <c r="B63" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C63" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D63" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E63" t="n">
-        <v>11884.0</v>
+        <v>4368.0</v>
       </c>
       <c r="F63" t="n">
-        <v>11884.0</v>
+        <v>4368.0</v>
       </c>
       <c r="G63" t="n">
-        <v>1.0881787382107866</v>
+        <v>1.006219765031099</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B64" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C64" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D64" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E64" t="n">
-        <v>10921.0</v>
+        <v>4341.0</v>
       </c>
       <c r="F64" t="n">
-        <v>10921.0</v>
+        <v>4341.0</v>
       </c>
       <c r="G64" t="n">
         <v>1.0</v>
@@ -3837,25 +3785,25 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B65" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C65" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D65" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E65" t="n">
-        <v>4368.0</v>
+        <v>6784.0</v>
       </c>
       <c r="F65" t="n">
-        <v>4368.0</v>
+        <v>6784.0</v>
       </c>
       <c r="G65" t="n">
-        <v>1.006219765031099</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="66">
@@ -3863,19 +3811,19 @@
         <v>26</v>
       </c>
       <c r="B66" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="C66" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D66" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E66" t="n">
-        <v>4341.0</v>
+        <v>5504.0</v>
       </c>
       <c r="F66" t="n">
-        <v>4341.0</v>
+        <v>5504.0</v>
       </c>
       <c r="G66" t="n">
         <v>1.0</v>
@@ -3883,22 +3831,22 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B67" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="C67" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D67" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E67" t="n">
-        <v>6784.0</v>
+        <v>8618.0</v>
       </c>
       <c r="F67" t="n">
-        <v>6784.0</v>
+        <v>8618.0</v>
       </c>
       <c r="G67" t="n">
         <v>1.0</v>
@@ -3906,25 +3854,25 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B68" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C68" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D68" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E68" t="n">
-        <v>5504.0</v>
+        <v>8916.0</v>
       </c>
       <c r="F68" t="n">
-        <v>5504.0</v>
+        <v>8916.0</v>
       </c>
       <c r="G68" t="n">
-        <v>1.0</v>
+        <v>3.884967320261438</v>
       </c>
     </row>
     <row r="69">
@@ -3932,19 +3880,19 @@
         <v>27</v>
       </c>
       <c r="B69" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="C69" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D69" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E69" t="n">
-        <v>8618.0</v>
+        <v>2295.0</v>
       </c>
       <c r="F69" t="n">
-        <v>8618.0</v>
+        <v>2295.0</v>
       </c>
       <c r="G69" t="n">
         <v>1.0</v>
@@ -3952,45 +3900,45 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B70" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C70" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D70" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E70" t="n">
-        <v>8916.0</v>
+        <v>2480.0</v>
       </c>
       <c r="F70" t="n">
-        <v>8916.0</v>
+        <v>2480.0</v>
       </c>
       <c r="G70" t="n">
-        <v>3.884967320261438</v>
+        <v>0.3990345937248592</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B71" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C71" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D71" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E71" t="n">
-        <v>2295.0</v>
+        <v>6215.0</v>
       </c>
       <c r="F71" t="n">
-        <v>2295.0</v>
+        <v>6215.0</v>
       </c>
       <c r="G71" t="n">
         <v>1.0</v>
@@ -4001,42 +3949,42 @@
         <v>28</v>
       </c>
       <c r="B72" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C72" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D72" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E72" t="n">
-        <v>2480.0</v>
+        <v>2588.0</v>
       </c>
       <c r="F72" t="n">
-        <v>2480.0</v>
+        <v>2588.0</v>
       </c>
       <c r="G72" t="n">
-        <v>0.3990345937248592</v>
+        <v>1.4621468926553671</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B73" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C73" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D73" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E73" t="n">
-        <v>6215.0</v>
+        <v>1770.0</v>
       </c>
       <c r="F73" t="n">
-        <v>6215.0</v>
+        <v>1770.0</v>
       </c>
       <c r="G73" t="n">
         <v>1.0</v>
@@ -4044,25 +3992,25 @@
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B74" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C74" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D74" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E74" t="n">
-        <v>2588.0</v>
+        <v>2424.0</v>
       </c>
       <c r="F74" t="n">
-        <v>2588.0</v>
+        <v>2424.0</v>
       </c>
       <c r="G74" t="n">
-        <v>1.4621468926553671</v>
+        <v>0.17206132879045996</v>
       </c>
     </row>
     <row r="75">
@@ -4070,19 +4018,19 @@
         <v>29</v>
       </c>
       <c r="B75" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C75" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D75" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E75" t="n">
-        <v>1770.0</v>
+        <v>14088.0</v>
       </c>
       <c r="F75" t="n">
-        <v>1770.0</v>
+        <v>14088.0</v>
       </c>
       <c r="G75" t="n">
         <v>1.0</v>
@@ -4090,45 +4038,45 @@
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B76" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="C76" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D76" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E76" t="n">
-        <v>2424.0</v>
+        <v>1064.0</v>
       </c>
       <c r="F76" t="n">
-        <v>2424.0</v>
+        <v>1064.0</v>
       </c>
       <c r="G76" t="n">
-        <v>0.17206132879045996</v>
+        <v>1.1615720524017468</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B77" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="C77" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D77" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E77" t="n">
-        <v>14088.0</v>
+        <v>916.0</v>
       </c>
       <c r="F77" t="n">
-        <v>14088.0</v>
+        <v>916.0</v>
       </c>
       <c r="G77" t="n">
         <v>1.0</v>
@@ -4139,42 +4087,42 @@
         <v>30</v>
       </c>
       <c r="B78" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C78" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D78" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E78" t="n">
-        <v>1064.0</v>
+        <v>2500.0</v>
       </c>
       <c r="F78" t="n">
-        <v>1064.0</v>
+        <v>2500.0</v>
       </c>
       <c r="G78" t="n">
-        <v>1.1615720524017468</v>
+        <v>0.7886435331230284</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B79" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C79" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D79" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E79" t="n">
-        <v>916.0</v>
+        <v>3170.0</v>
       </c>
       <c r="F79" t="n">
-        <v>916.0</v>
+        <v>3170.0</v>
       </c>
       <c r="G79" t="n">
         <v>1.0</v>
@@ -4182,25 +4130,25 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B80" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="C80" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D80" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E80" t="n">
-        <v>2500.0</v>
+        <v>1216.0</v>
       </c>
       <c r="F80" t="n">
-        <v>2500.0</v>
+        <v>1216.0</v>
       </c>
       <c r="G80" t="n">
-        <v>0.7886435331230284</v>
+        <v>0.37197919853166106</v>
       </c>
     </row>
     <row r="81">
@@ -4208,19 +4156,19 @@
         <v>31</v>
       </c>
       <c r="B81" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="C81" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D81" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E81" t="n">
-        <v>3170.0</v>
+        <v>3269.0</v>
       </c>
       <c r="F81" t="n">
-        <v>3170.0</v>
+        <v>3269.0</v>
       </c>
       <c r="G81" t="n">
         <v>1.0</v>
@@ -4228,93 +4176,47 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B82" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="C82" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D82" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E82" t="n">
-        <v>1216.0</v>
+        <v>1488.0</v>
       </c>
       <c r="F82" t="n">
-        <v>1216.0</v>
+        <v>1488.0</v>
       </c>
       <c r="G82" t="n">
-        <v>0.37197919853166106</v>
+        <v>0.36895611207537815</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B83" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="C83" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D83" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E83" t="n">
-        <v>3269.0</v>
+        <v>4033.0</v>
       </c>
       <c r="F83" t="n">
-        <v>3269.0</v>
+        <v>4033.0</v>
       </c>
       <c r="G83" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="s">
-        <v>32</v>
-      </c>
-      <c r="B84" t="s">
-        <v>121</v>
-      </c>
-      <c r="C84" t="s">
-        <v>91</v>
-      </c>
-      <c r="D84" t="s">
-        <v>196</v>
-      </c>
-      <c r="E84" t="n">
-        <v>1488.0</v>
-      </c>
-      <c r="F84" t="n">
-        <v>1488.0</v>
-      </c>
-      <c r="G84" t="n">
-        <v>0.36895611207537815</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="s">
-        <v>195</v>
-      </c>
-      <c r="B85" t="s">
-        <v>121</v>
-      </c>
-      <c r="C85" t="s">
-        <v>90</v>
-      </c>
-      <c r="D85" t="s">
-        <v>196</v>
-      </c>
-      <c r="E85" t="n">
-        <v>4033.0</v>
-      </c>
-      <c r="F85" t="n">
-        <v>4033.0</v>
-      </c>
-      <c r="G85" t="n">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>